<commit_message>
added 20200731 data to burndown chart
</commit_message>
<xml_diff>
--- a/burndown/burndown.xlsx
+++ b/burndown/burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cabohn/courses/csce361/grading-hot-repos/capstone/36team2/burndown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B0966C-FA66-9345-92A8-727B3637E458}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CAD073-12F0-FF49-9476-045A901B8A84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-1840" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 Burndown Chart" sheetId="2" r:id="rId1"/>
@@ -18,17 +18,6 @@
     <sheet name="Sprint 1 data" sheetId="1" r:id="rId3"/>
     <sheet name="Sprint 2 data" sheetId="3" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Sprint 1 data'!$A$2:$A$194</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Sprint 1 data'!$B$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Sprint 1 data'!$B$2:$B$194</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Sprint 1 data'!$C$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Sprint 1 data'!$C$2:$C$194</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Sprint 1 data'!$D$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Sprint 1 data'!$D$2:$D$194</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Sprint 1 data'!$E$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Sprint 1 data'!$E$2:$E$194</definedName>
-  </definedNames>
   <calcPr calcId="181029" concurrentCalc="0"/>
 </workbook>
 </file>
@@ -11470,7 +11459,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="242" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="153" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11492,7 +11481,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8669587" cy="6281777"/>
+    <xdr:ext cx="8674183" cy="6291895"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">

</xml_diff>

<commit_message>
added 20200801 data to burndown chart
</commit_message>
<xml_diff>
--- a/burndown/burndown.xlsx
+++ b/burndown/burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cabohn/courses/csce361/grading-hot-repos/capstone/36team2/burndown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CAD073-12F0-FF49-9476-045A901B8A84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB3DC82-A25F-6041-A0C8-60D332179296}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 Burndown Chart" sheetId="2" r:id="rId1"/>
@@ -11842,7 +11842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G194"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A54" workbookViewId="0">
       <selection sqref="A1:D194"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added 20200802 data to burndown chart
</commit_message>
<xml_diff>
--- a/burndown/burndown.xlsx
+++ b/burndown/burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cabohn/courses/csce361/grading-hot-repos/capstone/36team2/burndown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB3DC82-A25F-6041-A0C8-60D332179296}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EDE006-ED07-0F48-A8DC-95FBA88E4B35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-88460" yWindow="3380" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 Burndown Chart" sheetId="2" r:id="rId1"/>
@@ -11459,7 +11459,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="153" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="152" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11481,7 +11481,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8674183" cy="6291895"/>
+    <xdr:ext cx="8672763" cy="6291513"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11842,7 +11842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G194"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D194"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added 20200803 data to burndown chart
</commit_message>
<xml_diff>
--- a/burndown/burndown.xlsx
+++ b/burndown/burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cabohn/courses/csce361/grading-hot-repos/capstone/36team2/burndown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EDE006-ED07-0F48-A8DC-95FBA88E4B35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C6D911-2A73-1548-B84E-2B383B3C527A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-88460" yWindow="3380" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-44340" yWindow="2340" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 Burndown Chart" sheetId="2" r:id="rId1"/>
@@ -2917,100 +2917,100 @@
                   <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>37</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11842,8 +11842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G194"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D194"/>
+    <sheetView topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="A163" sqref="A163:D194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14775,7 +14775,7 @@
         <v>165</v>
       </c>
       <c r="B163">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -14785,7 +14785,7 @@
       </c>
       <c r="G163">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
@@ -14793,7 +14793,7 @@
         <v>166</v>
       </c>
       <c r="B164">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -14803,7 +14803,7 @@
       </c>
       <c r="G164">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
@@ -14811,7 +14811,7 @@
         <v>167</v>
       </c>
       <c r="B165">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -14821,7 +14821,7 @@
       </c>
       <c r="G165">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
@@ -14829,7 +14829,7 @@
         <v>168</v>
       </c>
       <c r="B166">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C166">
         <v>0</v>
@@ -14839,7 +14839,7 @@
       </c>
       <c r="G166">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
@@ -14847,7 +14847,7 @@
         <v>169</v>
       </c>
       <c r="B167">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C167">
         <v>0</v>
@@ -14857,7 +14857,7 @@
       </c>
       <c r="G167">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
@@ -14865,7 +14865,7 @@
         <v>170</v>
       </c>
       <c r="B168">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C168">
         <v>0</v>
@@ -14875,7 +14875,7 @@
       </c>
       <c r="G168">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
@@ -14883,7 +14883,7 @@
         <v>171</v>
       </c>
       <c r="B169">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C169">
         <v>0</v>
@@ -14893,7 +14893,7 @@
       </c>
       <c r="G169">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
@@ -14901,7 +14901,7 @@
         <v>172</v>
       </c>
       <c r="B170">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C170">
         <v>0</v>
@@ -14911,7 +14911,7 @@
       </c>
       <c r="G170">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
@@ -14919,7 +14919,7 @@
         <v>173</v>
       </c>
       <c r="B171">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C171">
         <v>0</v>
@@ -14929,7 +14929,7 @@
       </c>
       <c r="G171">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
@@ -14937,7 +14937,7 @@
         <v>174</v>
       </c>
       <c r="B172">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C172">
         <v>0</v>
@@ -14947,7 +14947,7 @@
       </c>
       <c r="G172">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
@@ -14955,7 +14955,7 @@
         <v>175</v>
       </c>
       <c r="B173">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C173">
         <v>0</v>
@@ -14965,7 +14965,7 @@
       </c>
       <c r="G173">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
@@ -14973,7 +14973,7 @@
         <v>176</v>
       </c>
       <c r="B174">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C174">
         <v>0</v>
@@ -14983,7 +14983,7 @@
       </c>
       <c r="G174">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
@@ -14991,7 +14991,7 @@
         <v>177</v>
       </c>
       <c r="B175">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C175">
         <v>0</v>
@@ -15001,7 +15001,7 @@
       </c>
       <c r="G175">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
@@ -15009,7 +15009,7 @@
         <v>178</v>
       </c>
       <c r="B176">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C176">
         <v>0</v>
@@ -15019,7 +15019,7 @@
       </c>
       <c r="G176">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
@@ -15027,7 +15027,7 @@
         <v>179</v>
       </c>
       <c r="B177">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C177">
         <v>0</v>
@@ -15037,7 +15037,7 @@
       </c>
       <c r="G177">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
@@ -15045,7 +15045,7 @@
         <v>180</v>
       </c>
       <c r="B178">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C178">
         <v>0</v>
@@ -15055,7 +15055,7 @@
       </c>
       <c r="G178">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
@@ -15063,7 +15063,7 @@
         <v>181</v>
       </c>
       <c r="B179">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C179">
         <v>0</v>
@@ -15073,7 +15073,7 @@
       </c>
       <c r="G179">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.2">
@@ -15081,7 +15081,7 @@
         <v>182</v>
       </c>
       <c r="B180">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C180">
         <v>0</v>
@@ -15091,7 +15091,7 @@
       </c>
       <c r="G180">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
@@ -15099,7 +15099,7 @@
         <v>183</v>
       </c>
       <c r="B181">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C181">
         <v>0</v>
@@ -15109,7 +15109,7 @@
       </c>
       <c r="G181">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
@@ -15117,7 +15117,7 @@
         <v>184</v>
       </c>
       <c r="B182">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C182">
         <v>0</v>
@@ -15127,7 +15127,7 @@
       </c>
       <c r="G182">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
@@ -15135,7 +15135,7 @@
         <v>185</v>
       </c>
       <c r="B183">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C183">
         <v>0</v>
@@ -15145,7 +15145,7 @@
       </c>
       <c r="G183">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
@@ -15153,7 +15153,7 @@
         <v>186</v>
       </c>
       <c r="B184">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C184">
         <v>0</v>
@@ -15163,7 +15163,7 @@
       </c>
       <c r="G184">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
@@ -15171,7 +15171,7 @@
         <v>187</v>
       </c>
       <c r="B185">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C185">
         <v>0</v>
@@ -15181,7 +15181,7 @@
       </c>
       <c r="G185">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
@@ -15189,7 +15189,7 @@
         <v>188</v>
       </c>
       <c r="B186">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C186">
         <v>0</v>
@@ -15199,7 +15199,7 @@
       </c>
       <c r="G186">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
@@ -15207,7 +15207,7 @@
         <v>189</v>
       </c>
       <c r="B187">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C187">
         <v>0</v>
@@ -15217,7 +15217,7 @@
       </c>
       <c r="G187">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
@@ -15225,7 +15225,7 @@
         <v>190</v>
       </c>
       <c r="B188">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C188">
         <v>0</v>
@@ -15235,7 +15235,7 @@
       </c>
       <c r="G188">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
@@ -15243,7 +15243,7 @@
         <v>191</v>
       </c>
       <c r="B189">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C189">
         <v>0</v>
@@ -15253,7 +15253,7 @@
       </c>
       <c r="G189">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
@@ -15261,7 +15261,7 @@
         <v>192</v>
       </c>
       <c r="B190">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C190">
         <v>0</v>
@@ -15271,7 +15271,7 @@
       </c>
       <c r="G190">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
@@ -15279,7 +15279,7 @@
         <v>193</v>
       </c>
       <c r="B191">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C191">
         <v>0</v>
@@ -15289,7 +15289,7 @@
       </c>
       <c r="G191">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.2">
@@ -15297,7 +15297,7 @@
         <v>194</v>
       </c>
       <c r="B192">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C192">
         <v>0</v>
@@ -15307,7 +15307,7 @@
       </c>
       <c r="G192">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.2">
@@ -15315,7 +15315,7 @@
         <v>195</v>
       </c>
       <c r="B193">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C193">
         <v>0</v>
@@ -15325,7 +15325,7 @@
       </c>
       <c r="G193">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.2">
@@ -15333,7 +15333,7 @@
         <v>196</v>
       </c>
       <c r="B194">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C194">
         <v>0</v>
@@ -15346,7 +15346,7 @@
       </c>
       <c r="G194">
         <f>SUM(B194:E194)</f>
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 20200804 data to burndown chart, concluding spring 1 burndown
</commit_message>
<xml_diff>
--- a/burndown/burndown.xlsx
+++ b/burndown/burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cabohn/courses/csce361/grading-hot-repos/capstone/36team2/burndown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C6D911-2A73-1548-B84E-2B383B3C527A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2482677-2F3F-F949-A04E-CFB6DF371C31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44340" yWindow="2340" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-86420" yWindow="1960" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 Burndown Chart" sheetId="2" r:id="rId1"/>
@@ -3001,16 +3001,16 @@
                   <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>34</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>34</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>34</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>34</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5409,16 +5409,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>1</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11842,8 +11842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G194"/>
   <sheetViews>
-    <sheetView topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="A163" sqref="A163:D194"/>
+    <sheetView topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="B194" sqref="B194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15279,13 +15279,13 @@
         <v>193</v>
       </c>
       <c r="B191">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C191">
         <v>0</v>
       </c>
       <c r="D191">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G191">
         <f t="shared" si="2"/>
@@ -15297,13 +15297,13 @@
         <v>194</v>
       </c>
       <c r="B192">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C192">
         <v>0</v>
       </c>
       <c r="D192">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="G192">
         <f t="shared" si="2"/>
@@ -15315,13 +15315,13 @@
         <v>195</v>
       </c>
       <c r="B193">
+        <v>1</v>
+      </c>
+      <c r="C193">
+        <v>0</v>
+      </c>
+      <c r="D193">
         <v>34</v>
-      </c>
-      <c r="C193">
-        <v>0</v>
-      </c>
-      <c r="D193">
-        <v>1</v>
       </c>
       <c r="G193">
         <f t="shared" si="2"/>
@@ -15333,20 +15333,20 @@
         <v>196</v>
       </c>
       <c r="B194">
+        <v>0</v>
+      </c>
+      <c r="C194">
+        <v>0</v>
+      </c>
+      <c r="D194">
         <v>34</v>
-      </c>
-      <c r="C194">
-        <v>0</v>
-      </c>
-      <c r="D194">
-        <v>1</v>
       </c>
       <c r="E194">
         <v>0</v>
       </c>
       <c r="G194">
         <f>SUM(B194:E194)</f>
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated burndown chart with 20200809 data
</commit_message>
<xml_diff>
--- a/burndown/burndown.xlsx
+++ b/burndown/burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cabohn/courses/csce361/grading-hot-repos/capstone/36team2/burndown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF10FE6-674D-A64E-84D8-87E3BE9C4737}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA2F58A-3317-D947-86B5-6420BFB1513D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-86420" yWindow="1960" windowWidth="33600" windowHeight="19280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35560" yWindow="-3680" windowWidth="33600" windowHeight="19280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 Burndown Chart" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
updated burndown charts with 20200811 data
</commit_message>
<xml_diff>
--- a/burndown/burndown.xlsx
+++ b/burndown/burndown.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cabohn/courses/csce361/grading-hot-repos/capstone/36team2/burndown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86539B54-8A6B-7443-B644-C587816DE0F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2158B71D-D8A0-4E41-B9CE-3CC10194D9B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35560" yWindow="-3680" windowWidth="33600" windowHeight="19280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
updated burndown charts with end-of-project data
</commit_message>
<xml_diff>
--- a/burndown/burndown.xlsx
+++ b/burndown/burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cabohn/courses/csce361/grading-hot-repos/capstone/36team2/burndown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2158B71D-D8A0-4E41-B9CE-3CC10194D9B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05428104-789F-3A49-BB08-4BE2E16E613A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35560" yWindow="-3680" windowWidth="33600" windowHeight="19280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7003,16 +7003,16 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>31</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>31</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>31</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>31</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9411,16 +9411,16 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>4</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>4</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>4</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>4</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18795,13 +18795,13 @@
         <v>202</v>
       </c>
       <c r="B191">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C191">
         <v>0</v>
       </c>
       <c r="D191">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G191">
         <f t="shared" si="2"/>
@@ -18813,13 +18813,13 @@
         <v>201</v>
       </c>
       <c r="B192">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C192">
         <v>0</v>
       </c>
       <c r="D192">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G192">
         <f t="shared" si="2"/>
@@ -18831,13 +18831,13 @@
         <v>200</v>
       </c>
       <c r="B193">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C193">
         <v>0</v>
       </c>
       <c r="D193">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G193">
         <f t="shared" si="2"/>
@@ -18849,13 +18849,13 @@
         <v>199</v>
       </c>
       <c r="B194">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C194">
         <v>0</v>
       </c>
       <c r="D194">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E194">
         <v>0</v>

</xml_diff>